<commit_message>
Balanco de potencias feito
</commit_message>
<xml_diff>
--- a/Balanço_Potências.xlsx
+++ b/Balanço_Potências.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\OneDrive\Ambiente de Trabalho\pie2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/a82090_uminho_pt/Documents/PIE2/PIE2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62551760-4960-49D0-9395-423DE962E6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{C611E25C-2B07-4838-AFB0-047B1456E501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D7D6B44-0626-4774-BB55-E535A3BFC254}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B980EE51-CC39-46DE-8223-2CCEEC94C929}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B980EE51-CC39-46DE-8223-2CCEEC94C929}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="30">
   <si>
     <t>Lote</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Comercio - Estabelecimento comercial</t>
-  </si>
-  <si>
-    <t>Aparcamento</t>
   </si>
   <si>
     <t>L1</t>
@@ -113,16 +110,39 @@
   </si>
   <si>
     <t>Pisos(1 ao 4)</t>
+  </si>
+  <si>
+    <t>T3 Power (KVA)</t>
+  </si>
+  <si>
+    <t>Aparcamento/ S.C.</t>
+  </si>
+  <si>
+    <t>Serviços Comuns 
+(S.C)</t>
+  </si>
+  <si>
+    <t>Charging Station 
+Power ( KW ) (Coletivo)</t>
+  </si>
+  <si>
+    <t>Fatores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,8 +168,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -157,16 +180,41 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -177,6 +225,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44E0C8AA-479C-460B-8AE2-BFB5813C9E4F}" name="Tabela1" displayName="Tabela1" ref="B2:H22" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="B2:H22" xr:uid="{44E0C8AA-479C-460B-8AE2-BFB5813C9E4F}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{5887296E-0848-4CF9-A77C-58E87A846C1A}" name="Lote" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{EC41635C-0445-4037-805E-7A7A23CBFBDD}" name="Tipo" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{59BB85CB-4B97-455F-B21B-9D7479D37280}" name="Pisos" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{5FB4D7F4-D0F8-402C-ABC0-EF1370863CED}" name="Caracterização" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{64F829D4-E957-44FE-95C1-36C7DA27A857}" name="Numero" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{67AC4821-53B6-4945-B5D3-7830BBB3C51B}" name="Potencia(KVA)" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{C11431A9-5825-4149-96CC-E56ED627CB14}" name="Potência Total por Lote" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -476,22 +540,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC4E119-E615-4786-A97F-B3A0412982D4}">
-  <dimension ref="B2:H23"/>
+  <dimension ref="B2:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" customWidth="1"/>
-    <col min="8" max="8" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="13" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -508,459 +575,507 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <f>L3 + J3</f>
+        <v>25.45</v>
+      </c>
+      <c r="H3" s="2">
+        <f>G5+G4+G3</f>
+        <v>132.39999999999998</v>
+      </c>
+      <c r="J3">
+        <v>3.45</v>
+      </c>
+      <c r="K3">
+        <v>7.2</v>
+      </c>
+      <c r="L3">
+        <v>22</v>
+      </c>
+      <c r="M3">
+        <f>10.35</f>
+        <v>10.35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
-        <f>3*10.35</f>
-        <v>31.049999999999997</v>
-      </c>
-      <c r="H3" s="1">
-        <f>G5+G4+G3</f>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f>F4*6.9</f>
         <v>13.8</v>
       </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3" t="s">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>9</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f>F5*10.35</f>
         <v>93.149999999999991</v>
       </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="G6" s="3">
-        <f>3*10.35</f>
-        <v>31.049999999999997</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="G6" s="2">
+        <f>L3 + J3</f>
+        <v>25.45</v>
+      </c>
+      <c r="H6" s="2">
         <f t="shared" ref="H6" si="0">G8+G7+G6</f>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3" t="s">
+        <v>132.39999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>2</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <f>F4*6.9</f>
         <v>13.8</v>
       </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3" t="s">
+      <c r="H7" s="2"/>
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>9</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <f>F8*10.35</f>
         <v>93.149999999999991</v>
       </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="2">
         <v>1</v>
       </c>
-      <c r="G9" s="3">
-        <f>5*10.35</f>
-        <v>51.75</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="G9" s="2">
+        <f>L3 + J3</f>
+        <v>25.45</v>
+      </c>
+      <c r="H9" s="2">
         <f t="shared" ref="H9" si="1">G11+G10+G9</f>
-        <v>175.95</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3" t="s">
+        <v>149.64999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>3</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <f>F10*10.35</f>
         <v>31.049999999999997</v>
       </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3" t="s">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>9</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <f>F11*10.35</f>
         <v>93.149999999999991</v>
       </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="3">
+      <c r="E12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="2">
         <v>1</v>
       </c>
-      <c r="G12" s="3">
-        <f>5*10.35</f>
-        <v>51.75</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="G12" s="2">
+        <f>2*L3+J3</f>
+        <v>47.45</v>
+      </c>
+      <c r="H12" s="2">
         <f t="shared" ref="H12" si="2">G14+G13+G12</f>
-        <v>207</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3" t="s">
+        <v>202.7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>3</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <f>F13*10.35</f>
         <v>31.049999999999997</v>
       </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>12</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <f>F14*10.35</f>
         <v>124.19999999999999</v>
       </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="E15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="2">
         <v>1</v>
       </c>
-      <c r="G15" s="3">
-        <f>4*10.35</f>
-        <v>41.4</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="G15" s="2">
+        <f>2*L3+J3</f>
+        <v>47.45</v>
+      </c>
+      <c r="H15" s="2">
         <f t="shared" ref="H15" si="3">G17+G16+G15</f>
-        <v>196.65</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3" t="s">
+        <v>202.7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>2</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <f>F13*10.35</f>
         <v>31.049999999999997</v>
       </c>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>12</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
         <f>F17*10.35</f>
         <v>124.19999999999999</v>
       </c>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="3">
+      <c r="E18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="2">
         <v>1</v>
       </c>
-      <c r="G18" s="3">
-        <f>4*10.35</f>
-        <v>41.4</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="G18" s="2">
+        <f>2*L3+J3</f>
+        <v>47.45</v>
+      </c>
+      <c r="H18" s="2">
         <f t="shared" ref="H18" si="4">G20+G19+G18</f>
-        <v>179.4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3" t="s">
+        <v>185.45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>2</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <f>F4*6.9</f>
         <v>13.8</v>
       </c>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>12</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <f>F20*10.35</f>
         <v>124.19999999999999</v>
       </c>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="2">
+        <v>16</v>
+      </c>
+      <c r="G21" s="2">
+        <f>K3</f>
+        <v>7.2</v>
+      </c>
+      <c r="H21" s="2">
+        <f>(G22+G21)</f>
+        <v>17.55</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="2">
+        <v>16</v>
+      </c>
+      <c r="G22" s="2">
+        <v>10.35</v>
+      </c>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="3">
-        <v>1</v>
-      </c>
-      <c r="G21" s="3">
-        <f>10.35</f>
-        <v>10.35</v>
-      </c>
-      <c r="H21" s="1">
-        <f>(G22+G21)</f>
-        <v>20.7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-      <c r="G22" s="3">
-        <v>10.35</v>
-      </c>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="4">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="1">
         <f>H3+H9+H6+H12+H15+H18+(H21*16)</f>
-        <v>1366.2</v>
+        <v>1286.0999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f>SUM(F5:F20)</f>
+        <v>80</v>
+      </c>
+      <c r="G24">
+        <f>SUM(G21:G22)</f>
+        <v>17.55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="H21:H22"/>
+  <mergeCells count="1">
     <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>